<commit_message>
modification of sample names
</commit_message>
<xml_diff>
--- a/wing_discs.xlsx
+++ b/wing_discs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scheti00/PycharmProjects/Wingdisc-alignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA03EE8F-065E-274B-A19E-F5D3C459D7A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07176D8E-DECC-C04D-8B0F-92FCEEB1EB52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,13 +50,13 @@
     <t>7_9</t>
   </si>
   <si>
-    <t>Whateveryouwant</t>
-  </si>
-  <si>
     <t>Sample1</t>
   </si>
   <si>
     <t>Sampl2_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any Name </t>
   </si>
 </sst>
 </file>
@@ -1387,7 +1387,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>4</v>
@@ -11550,7 +11550,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>4</v>
@@ -15425,7 +15425,7 @@
   <dimension ref="A1:E538"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15435,7 +15435,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>4</v>

</xml_diff>